<commit_message>
Modified attendance sheets for next iterations
</commit_message>
<xml_diff>
--- a/FA17/MA122/AttendanceSheet001.xlsx
+++ b/FA17/MA122/AttendanceSheet001.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Documents\Teaching\FA17\MA122\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19665" windowHeight="14085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19660" windowHeight="14080"/>
   </bookViews>
   <sheets>
     <sheet name="AttendanceSheet001" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
   <si>
     <t>Aiken</t>
   </si>
@@ -388,12 +388,6 @@
   </si>
   <si>
     <t>JAMES</t>
-  </si>
-  <si>
-    <t>Wain</t>
-  </si>
-  <si>
-    <t>ALEXANDRA</t>
   </si>
   <si>
     <t>Walker</t>
@@ -431,7 +425,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -867,16 +861,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -927,8 +921,8 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1032,7 +1026,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1067,7 +1061,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1244,7 +1238,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1252,24 +1246,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O72"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="4" customWidth="1"/>
-    <col min="3" max="15" width="8.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="11.1640625" style="4" customWidth="1"/>
+    <col min="3" max="15" width="8.6640625" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1">
@@ -1312,7 +1306,7 @@
         <v>43014</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1333,7 +1327,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1354,7 +1348,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1375,7 +1369,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1396,7 +1390,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1417,7 +1411,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1438,7 +1432,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1459,7 +1453,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1480,7 +1474,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1501,7 +1495,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1522,7 +1516,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -1543,7 +1537,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1564,7 +1558,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1585,7 +1579,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1606,7 +1600,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1627,7 +1621,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
@@ -1648,7 +1642,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1669,7 +1663,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -1690,7 +1684,7 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -1711,7 +1705,7 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
@@ -1732,7 +1726,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
@@ -1753,7 +1747,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="3" t="s">
         <v>42</v>
       </c>
@@ -1774,7 +1768,7 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
@@ -1795,7 +1789,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
@@ -1816,7 +1810,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -1837,7 +1831,7 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
@@ -1858,7 +1852,7 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -1879,7 +1873,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="3" t="s">
         <v>54</v>
       </c>
@@ -1900,7 +1894,7 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="3" t="s">
         <v>56</v>
       </c>
@@ -1921,7 +1915,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
@@ -1942,7 +1936,7 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
@@ -1963,7 +1957,7 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="3" t="s">
         <v>62</v>
       </c>
@@ -1984,7 +1978,7 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="3" t="s">
         <v>64</v>
       </c>
@@ -2005,7 +1999,7 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="3" t="s">
         <v>66</v>
       </c>
@@ -2026,7 +2020,7 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="3" t="s">
         <v>68</v>
       </c>
@@ -2047,7 +2041,7 @@
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="3" t="s">
         <v>70</v>
       </c>
@@ -2068,7 +2062,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="3" t="s">
         <v>72</v>
       </c>
@@ -2089,7 +2083,7 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="3" t="s">
         <v>73</v>
       </c>
@@ -2110,7 +2104,7 @@
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="3" t="s">
         <v>75</v>
       </c>
@@ -2131,7 +2125,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" s="3" t="s">
         <v>77</v>
       </c>
@@ -2152,7 +2146,7 @@
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" s="3" t="s">
         <v>78</v>
       </c>
@@ -2173,7 +2167,7 @@
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" s="3" t="s">
         <v>80</v>
       </c>
@@ -2194,7 +2188,7 @@
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" s="3" t="s">
         <v>82</v>
       </c>
@@ -2215,7 +2209,7 @@
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" s="3" t="s">
         <v>84</v>
       </c>
@@ -2236,7 +2230,7 @@
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" s="3" t="s">
         <v>86</v>
       </c>
@@ -2257,7 +2251,7 @@
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" s="3" t="s">
         <v>88</v>
       </c>
@@ -2278,7 +2272,7 @@
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" s="3" t="s">
         <v>89</v>
       </c>
@@ -2299,7 +2293,7 @@
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" s="3" t="s">
         <v>91</v>
       </c>
@@ -2320,7 +2314,7 @@
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15">
       <c r="A50" s="3" t="s">
         <v>93</v>
       </c>
@@ -2341,7 +2335,7 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15">
       <c r="A51" s="3" t="s">
         <v>95</v>
       </c>
@@ -2362,7 +2356,7 @@
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" s="3" t="s">
         <v>97</v>
       </c>
@@ -2383,7 +2377,7 @@
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="A53" s="3" t="s">
         <v>99</v>
       </c>
@@ -2404,7 +2398,7 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15">
       <c r="A54" s="3" t="s">
         <v>101</v>
       </c>
@@ -2425,7 +2419,7 @@
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" s="3" t="s">
         <v>102</v>
       </c>
@@ -2446,7 +2440,7 @@
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15">
       <c r="A56" s="3" t="s">
         <v>104</v>
       </c>
@@ -2467,7 +2461,7 @@
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" s="3" t="s">
         <v>106</v>
       </c>
@@ -2488,7 +2482,7 @@
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15">
       <c r="A58" s="3" t="s">
         <v>108</v>
       </c>
@@ -2509,7 +2503,7 @@
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15">
       <c r="A59" s="3" t="s">
         <v>110</v>
       </c>
@@ -2530,7 +2524,7 @@
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15">
       <c r="A60" s="3" t="s">
         <v>112</v>
       </c>
@@ -2551,7 +2545,7 @@
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15">
       <c r="A61" s="3" t="s">
         <v>114</v>
       </c>
@@ -2572,7 +2566,7 @@
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15">
       <c r="A62" s="3" t="s">
         <v>116</v>
       </c>
@@ -2593,7 +2587,7 @@
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" s="3" t="s">
         <v>118</v>
       </c>
@@ -2614,7 +2608,7 @@
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" s="3" t="s">
         <v>118</v>
       </c>
@@ -2635,7 +2629,7 @@
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15">
       <c r="A65" s="3" t="s">
         <v>121</v>
       </c>
@@ -2656,7 +2650,7 @@
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15">
       <c r="A66" s="3" t="s">
         <v>123</v>
       </c>
@@ -2677,12 +2671,12 @@
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15">
       <c r="A67" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>126</v>
+        <v>63</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -2698,12 +2692,12 @@
       <c r="N67" s="3"/>
       <c r="O67" s="3"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15">
       <c r="A68" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -2719,7 +2713,7 @@
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15">
       <c r="A69" s="3" t="s">
         <v>128</v>
       </c>
@@ -2740,12 +2734,12 @@
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15">
       <c r="A70" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -2761,12 +2755,12 @@
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15">
       <c r="A71" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -2782,29 +2776,13 @@
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
-      <c r="N72" s="3"/>
-      <c r="O72" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+  <pageSetup scale="65" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>